<commit_message>
Presupuesto y circuitos preparados
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enner\Desktop\Clases\Tercer_a\PrimerSemestre\orga\lab\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0B57B9-F3EB-4691-AE53-C13C1031F731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832FEFDA-BC46-4B9A-B8DC-07413DE9BFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11DC2AD5-8071-4EE4-B263-3E3713044B80}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -90,6 +90,45 @@
   </si>
   <si>
     <t xml:space="preserve">DISPSWITCH </t>
+  </si>
+  <si>
+    <t>Masking Tape</t>
+  </si>
+  <si>
+    <t>2 placas cobre</t>
+  </si>
+  <si>
+    <t>20 TRANSISTORES  2N2222A</t>
+  </si>
+  <si>
+    <t>Esponja para limpiar punta de cautín</t>
+  </si>
+  <si>
+    <t>4 Terminal block 2 contactos</t>
+  </si>
+  <si>
+    <t>2 Terminal block 3 contactos</t>
+  </si>
+  <si>
+    <t>Dip switch 3 posiciones tipo integrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metro de estaño de 0.8mm </t>
+  </si>
+  <si>
+    <t>10 resistencias de 330 ohm</t>
+  </si>
+  <si>
+    <t>Cloruro férrico</t>
+  </si>
+  <si>
+    <t>30 resistencias de 1K ohm</t>
+  </si>
+  <si>
+    <t>2 metros de alambre para protoboard</t>
+  </si>
+  <si>
+    <t>2 impresiones en papel coshé</t>
   </si>
 </sst>
 </file>
@@ -99,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Q&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +166,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,15 +252,7 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,7 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -237,9 +277,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB57228-255D-439C-881D-1474A89D4AEE}">
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,356 +636,715 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>45691</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="1">
         <v>16.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="4">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="2">
         <f>SUM(G4:G9)</f>
         <v>89.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="13">
         <v>45693</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="4">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="2">
         <f>SUM(G11:G13)</f>
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="13">
         <v>45698</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="1">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="2">
         <f>SUM(G15:G18)</f>
         <v>68.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="1"/>
+      <c r="A20" s="13">
+        <v>45702</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="1"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="1"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="1"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="1"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="1"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="1"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
+      <c r="B33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="2">
+        <f>SUM(G20:G33)</f>
+        <v>145.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>45703</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="14"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="14"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="14"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="14"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="14"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="14"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="14"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="14"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="14"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="14"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="14"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="14"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="14"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="14"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="14"/>
+      <c r="B60" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="4">
-        <f>SUM(G10,G14,G19)</f>
-        <v>231</v>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="2">
+        <f>SUM(G10,G14,G19,G34)</f>
+        <v>376.6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B29:F29"/>
+  <mergeCells count="59">
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B2:G3"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
@@ -955,16 +1359,23 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización del presupuesto :(
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enner\Desktop\Clases\Tercer_a\PrimerSemestre\orga\lab\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832FEFDA-BC46-4B9A-B8DC-07413DE9BFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394D483-C145-4EE7-95E7-0B39D74135BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11DC2AD5-8071-4EE4-B263-3E3713044B80}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -129,6 +130,33 @@
   </si>
   <si>
     <t>2 impresiones en papel coshé</t>
+  </si>
+  <si>
+    <t>Lana abrasiva de acero</t>
+  </si>
+  <si>
+    <t>10 metros de alambre para protoboard</t>
+  </si>
+  <si>
+    <t>Dos placas de cobre</t>
+  </si>
+  <si>
+    <t>2 impresiones laser en papel fotografía</t>
+  </si>
+  <si>
+    <t>Lo de bryan</t>
+  </si>
+  <si>
+    <t>Lo de juanito</t>
+  </si>
+  <si>
+    <t>Lo del 14 en adelante</t>
+  </si>
+  <si>
+    <t>Acetona</t>
+  </si>
+  <si>
+    <t>Calculando lo que tendría que dar cada uno</t>
   </si>
 </sst>
 </file>
@@ -253,18 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,14 +295,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB57228-255D-439C-881D-1474A89D4AEE}">
-  <dimension ref="A2:G60"/>
+  <dimension ref="A2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,690 +659,730 @@
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
     <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="3">
         <v>45691</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="1">
         <v>16.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="2">
         <f>SUM(G4:G9)</f>
         <v>89.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="3">
         <v>45693</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="2">
         <f>SUM(G11:G13)</f>
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="3">
         <v>45698</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="2">
         <f>SUM(G15:G18)</f>
         <v>68.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
+      <c r="A20" s="3">
+        <v>45701</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>45702</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="1">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="1">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="1">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="1">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="1">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="1">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="1">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="1">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="6" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="1">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="6" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="1">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="6" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="1">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="6" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="1">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="G33" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="8" t="s">
-        <v>10</v>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="2">
-        <f>SUM(G20:G33)</f>
+      <c r="F34" s="9"/>
+      <c r="G34" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="2">
+        <f>SUM(G21:G34)</f>
         <v>145.6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>45703</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="B36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="2">
+        <f>SUM(G36:G39)</f>
+        <v>83</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="2">
+        <f>G60</f>
+        <v>494.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="14"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="14"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="14"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="14"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
       <c r="G60" s="2">
-        <f>SUM(G10,G14,G19,G34)</f>
-        <v>376.6</v>
+        <f>SUM(G10,G14,G19,G20,G35,G40)</f>
+        <v>494.6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
+    <mergeCell ref="I40:M40"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="B56:F56"/>
     <mergeCell ref="B57:F57"/>
@@ -1325,10 +1393,7 @@
     <mergeCell ref="B52:F52"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
@@ -1339,44 +1404,115 @@
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
     <mergeCell ref="B60:F60"/>
     <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B22:F22"/>
     <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B33:F33"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
     <mergeCell ref="B39:F39"/>
     <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0D60FF-52A3-4306-9349-507B8E75A23B}">
+  <dimension ref="B3:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <f>38.92/5</f>
+        <v>7.7840000000000007</v>
+      </c>
+      <c r="D7">
+        <v>38.92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <f>35/5</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <f>(145.6+83)/5</f>
+        <v>45.72</v>
+      </c>
+      <c r="D9">
+        <v>145.6</v>
+      </c>
+      <c r="E9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f>C7+C8+C9</f>
+        <v>60.503999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trabajo de anoche, 19 de febrero
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enner\Desktop\Clases\Tercer_a\PrimerSemestre\orga\lab\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B43E4-FF62-486B-B951-0FCA57201E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3923A7EE-6FB7-4A77-AEF7-726FAFF3E858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11DC2AD5-8071-4EE4-B263-3E3713044B80}"/>
+    <workbookView xWindow="2664" yWindow="2604" windowWidth="17280" windowHeight="9420" xr2:uid="{11DC2AD5-8071-4EE4-B263-3E3713044B80}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Brocas, impresiones, placas y componentes varios</t>
+  </si>
+  <si>
+    <t>Esponjas para limpiar cautín y estaño</t>
+  </si>
+  <si>
+    <t>Protoboard, resistencias de 100 ohmios y 10k</t>
   </si>
 </sst>
 </file>
@@ -289,19 +295,10 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -317,6 +314,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -655,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB57228-255D-439C-881D-1474A89D4AEE}">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,116 +676,116 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45691</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1">
         <v>16.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="2">
         <f>SUM(G4:G9)</f>
         <v>89.5</v>
@@ -789,52 +795,52 @@
       <c r="A11" s="3">
         <v>45693</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="2">
         <f>SUM(G11:G13)</f>
         <v>73</v>
@@ -844,65 +850,65 @@
       <c r="A15" s="3">
         <v>45698</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="2">
         <f>SUM(G15:G18)</f>
         <v>68.5</v>
@@ -912,13 +918,13 @@
       <c r="A20" s="3">
         <v>45701</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="2">
         <v>35</v>
       </c>
@@ -927,195 +933,195 @@
       <c r="A21" s="3">
         <v>45702</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="14"/>
       <c r="G35" s="2">
         <f>SUM(G21:G34)</f>
         <v>145.6</v>
@@ -1125,65 +1131,65 @@
       <c r="A36" s="3">
         <v>45703</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="2">
         <f>SUM(G36:G39)</f>
         <v>83</v>
@@ -1193,221 +1199,245 @@
       <c r="A41" s="3">
         <v>45705</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="1">
         <v>14.25</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="1">
         <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="2">
         <f>SUM(G41:G42)</f>
         <v>182.25</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="1"/>
+      <c r="A44" s="3">
+        <v>45706</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="1">
+        <v>28.5</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="1"/>
+      <c r="B45" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="1">
+        <v>41.5</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="1"/>
+      <c r="B46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="2">
+        <f>SUM(G44:G45)</f>
+        <v>70</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
       <c r="G60" s="2">
-        <f>SUM(G10,G14,G19,G20,G35,G40,G43)</f>
-        <v>676.85</v>
+        <f>SUM(G10,G14,G19,G20,G35,G40,G43,G46)</f>
+        <v>746.85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B2:G3"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
@@ -1424,32 +1454,23 @@
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B28:F28"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>